<commit_message>
Update Freeman Resource Guid Assigned Tabs.xlsx
</commit_message>
<xml_diff>
--- a/data/Freenman Center Resource Guide/Freeman Resource Guid Assigned Tabs.xlsx
+++ b/data/Freenman Center Resource Guide/Freeman Resource Guid Assigned Tabs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Hackathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathaniel\Documents\GitHub\NDoCH-2020\data\Freenman Center Resource Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B7F7A0-B5D7-43C5-847B-D2EA07DCEDCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE9DAA2-1D87-4653-8D54-35BF4650A05D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{718C3DC7-7001-4C06-8886-7191179CAEDD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{718C3DC7-7001-4C06-8886-7191179CAEDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>COVID - 19:   Community Updates</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>All of the ones in gray are done.</t>
+  </si>
+  <si>
+    <t>Nathaniel</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,6 +866,9 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B32" t="s">
         <v>29</v>
       </c>

</xml_diff>